<commit_message>
Updates to template and to output report.
* change output report to more closely resemble format of template
* update template file to add new properties
</commit_message>
<xml_diff>
--- a/resources/org/pharmgkb/ICPC_Submission_Template.xlsx
+++ b/resources/org/pharmgkb/ICPC_Submission_Template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pharmgkb_icpc\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1224" yWindow="264" windowWidth="16452" windowHeight="7164" tabRatio="500"/>
+    <workbookView xWindow="1170" yWindow="525" windowWidth="13830" windowHeight="5415" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -20,7 +25,7 @@
     <author>rcosenti</author>
   </authors>
   <commentList>
-    <comment ref="A42" authorId="0">
+    <comment ref="A42" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A98" authorId="0">
+    <comment ref="A98" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A124" authorId="0">
+    <comment ref="A124" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A136" authorId="0">
+    <comment ref="A136" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -121,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A137" authorId="0">
+    <comment ref="A137" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -145,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A138" authorId="0">
+    <comment ref="A138" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A245" authorId="0">
+    <comment ref="A245" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A249" authorId="0">
+    <comment ref="A249" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -227,7 +232,7 @@
     <author>rcosenti</author>
   </authors>
   <commentList>
-    <comment ref="Q2" authorId="0">
+    <comment ref="Q2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -251,7 +256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BU2" authorId="0">
+    <comment ref="BU2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -276,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CS2" authorId="0">
+    <comment ref="CS2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -304,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DE2" authorId="0">
+    <comment ref="DE2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -328,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DF2" authorId="0">
+    <comment ref="DF2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -352,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DG2" authorId="0">
+    <comment ref="DG2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -376,7 +381,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="HG2" authorId="0">
+    <comment ref="HG2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="356">
   <si>
     <t>Ever Smoked</t>
     <phoneticPr fontId="12" type="noConversion"/>
@@ -1488,6 +1493,48 @@
   </si>
   <si>
     <t xml:space="preserve">VASP assay, please try to specify whether it's after loading dose or maintenance dose. If not known, enter value here. Assay result  (numeric), expressed as a Platelet Reactivity Index (PRI) in % </t>
+  </si>
+  <si>
+    <t>VASP phosphorylation assay at baseline</t>
+  </si>
+  <si>
+    <t>Multiplate ADP post loading</t>
+  </si>
+  <si>
+    <t>Hypercholesterolemia</t>
+  </si>
+  <si>
+    <t>Non-target vessel revascularization</t>
+  </si>
+  <si>
+    <t>Time to the first hemorrhargic stroke</t>
+  </si>
+  <si>
+    <t>active malignancy</t>
+  </si>
+  <si>
+    <t>cardiogenic shock at the time of PCI</t>
+  </si>
+  <si>
+    <t>hemorrhargic stroke</t>
+  </si>
+  <si>
+    <t>peripheral arterial disease at baseline</t>
+  </si>
+  <si>
+    <t>stent type</t>
+  </si>
+  <si>
+    <t>target vessel revascularization</t>
+  </si>
+  <si>
+    <t>time to the first non-target vessel revascularization</t>
+  </si>
+  <si>
+    <t>time to the first target vessel revascularization</t>
+  </si>
+  <si>
+    <t>type of stent thrombosis</t>
   </si>
 </sst>
 </file>
@@ -16777,6 +16824,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -17105,15 +17155,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+    <sheetView topLeftCell="A228" workbookViewId="0">
       <selection activeCell="A232" sqref="A232"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="72.88671875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="70.6640625" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="10.6640625" style="11"/>
+    <col min="1" max="1" width="72.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" style="11" customWidth="1"/>
+    <col min="3" max="16384" width="10.7109375" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -17216,7 +17266,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="31.2">
+    <row r="15" spans="1:2" ht="31.5">
       <c r="A15" s="1" t="s">
         <v>103</v>
       </c>
@@ -17512,7 +17562,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="31.2">
+    <row r="55" spans="1:2" ht="31.5">
       <c r="A55" s="24" t="s">
         <v>222</v>
       </c>
@@ -17712,7 +17762,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="31.2">
+    <row r="80" spans="1:2" ht="31.5">
       <c r="A80" s="41" t="s">
         <v>263</v>
       </c>
@@ -17776,7 +17826,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="31.2">
+    <row r="88" spans="1:4" ht="31.5">
       <c r="A88" s="41" t="s">
         <v>272</v>
       </c>
@@ -17811,7 +17861,7 @@
       </c>
       <c r="C91" s="20"/>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" ht="31.5">
       <c r="A92" s="27" t="s">
         <v>163</v>
       </c>
@@ -17821,7 +17871,7 @@
       <c r="C92" s="20"/>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:4" ht="31.2">
+    <row r="93" spans="1:4" ht="31.5">
       <c r="A93" s="27" t="s">
         <v>229</v>
       </c>
@@ -17976,7 +18026,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="43.2">
+    <row r="111" spans="1:4" ht="45">
       <c r="A111" s="56" t="s">
         <v>306</v>
       </c>
@@ -17984,7 +18034,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="28.8">
+    <row r="112" spans="1:4" ht="45">
       <c r="A112" s="57" t="s">
         <v>307</v>
       </c>
@@ -18040,7 +18090,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="31.2">
+    <row r="119" spans="1:2" ht="31.5">
       <c r="A119" s="41" t="s">
         <v>171</v>
       </c>
@@ -18288,7 +18338,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" ht="31.5">
       <c r="A151" s="13" t="s">
         <v>76</v>
       </c>
@@ -18296,7 +18346,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" ht="31.5">
       <c r="A152" s="13" t="s">
         <v>77</v>
       </c>
@@ -18304,7 +18354,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="31.2">
+    <row r="153" spans="1:2" ht="31.5">
       <c r="A153" s="13" t="s">
         <v>78</v>
       </c>
@@ -18312,7 +18362,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="31.2">
+    <row r="154" spans="1:2" ht="31.5">
       <c r="A154" s="13" t="s">
         <v>212</v>
       </c>
@@ -18320,7 +18370,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="31.2">
+    <row r="155" spans="1:2" ht="31.5">
       <c r="A155" s="13" t="s">
         <v>301</v>
       </c>
@@ -18328,7 +18378,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="31.2">
+    <row r="156" spans="1:2" ht="31.5">
       <c r="A156" s="13" t="s">
         <v>302</v>
       </c>
@@ -18336,7 +18386,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="31.2">
+    <row r="157" spans="1:2" ht="31.5">
       <c r="A157" s="13" t="s">
         <v>303</v>
       </c>
@@ -18344,7 +18394,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="31.2">
+    <row r="158" spans="1:2" ht="31.5">
       <c r="A158" s="13" t="s">
         <v>172</v>
       </c>
@@ -18352,7 +18402,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="31.2">
+    <row r="159" spans="1:2" ht="31.5">
       <c r="A159" s="13" t="s">
         <v>173</v>
       </c>
@@ -18360,7 +18410,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="31.2">
+    <row r="160" spans="1:2" ht="31.5">
       <c r="A160" s="13" t="s">
         <v>174</v>
       </c>
@@ -18368,7 +18418,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="31.2">
+    <row r="161" spans="1:2" ht="31.5">
       <c r="A161" s="13" t="s">
         <v>175</v>
       </c>
@@ -18376,7 +18426,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="31.2">
+    <row r="162" spans="1:2" ht="31.5">
       <c r="A162" s="13" t="s">
         <v>179</v>
       </c>
@@ -18384,7 +18434,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="31.2">
+    <row r="163" spans="1:2" ht="31.5">
       <c r="A163" s="13" t="s">
         <v>180</v>
       </c>
@@ -18392,7 +18442,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="31.2">
+    <row r="164" spans="1:2" ht="31.5">
       <c r="A164" s="13" t="s">
         <v>181</v>
       </c>
@@ -18400,7 +18450,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="31.2">
+    <row r="165" spans="1:2" ht="31.5">
       <c r="A165" s="13" t="s">
         <v>182</v>
       </c>
@@ -18416,7 +18466,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="31.2">
+    <row r="167" spans="1:2" ht="31.5">
       <c r="A167" s="13" t="s">
         <v>80</v>
       </c>
@@ -18424,7 +18474,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" ht="31.5">
       <c r="A168" s="13" t="s">
         <v>183</v>
       </c>
@@ -18432,7 +18482,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" ht="31.5">
       <c r="A169" s="13" t="s">
         <v>184</v>
       </c>
@@ -18440,7 +18490,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" ht="31.5">
       <c r="A170" s="13" t="s">
         <v>185</v>
       </c>
@@ -18448,7 +18498,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" ht="31.5">
       <c r="A171" s="13" t="s">
         <v>186</v>
       </c>
@@ -18456,7 +18506,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="31.2">
+    <row r="172" spans="1:2" ht="31.5">
       <c r="A172" s="13" t="s">
         <v>242</v>
       </c>
@@ -18464,7 +18514,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="31.2">
+    <row r="173" spans="1:2" ht="31.5">
       <c r="A173" s="13" t="s">
         <v>178</v>
       </c>
@@ -18472,7 +18522,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="31.2">
+    <row r="174" spans="1:2" ht="31.5">
       <c r="A174" s="13" t="s">
         <v>243</v>
       </c>
@@ -18480,7 +18530,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="31.2">
+    <row r="175" spans="1:2" ht="31.5">
       <c r="A175" s="13" t="s">
         <v>244</v>
       </c>
@@ -18488,7 +18538,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="31.2">
+    <row r="176" spans="1:2" ht="31.5">
       <c r="A176" s="13" t="s">
         <v>245</v>
       </c>
@@ -18520,7 +18570,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="31.2">
+    <row r="180" spans="1:2" ht="31.5">
       <c r="A180" s="13" t="s">
         <v>81</v>
       </c>
@@ -18560,7 +18610,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="31.2">
+    <row r="185" spans="1:2" ht="31.5">
       <c r="A185" s="13" t="s">
         <v>252</v>
       </c>
@@ -18568,7 +18618,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="31.2">
+    <row r="186" spans="1:2" ht="31.5">
       <c r="A186" s="13" t="s">
         <v>211</v>
       </c>
@@ -18576,7 +18626,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="31.2">
+    <row r="187" spans="1:2" ht="31.5">
       <c r="A187" s="13" t="s">
         <v>276</v>
       </c>
@@ -18584,7 +18634,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="31.2">
+    <row r="188" spans="1:2" ht="31.5">
       <c r="A188" s="13" t="s">
         <v>277</v>
       </c>
@@ -18592,7 +18642,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="31.2">
+    <row r="189" spans="1:2" ht="31.5">
       <c r="A189" s="13" t="s">
         <v>278</v>
       </c>
@@ -18600,7 +18650,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="31.2">
+    <row r="190" spans="1:2" ht="31.5">
       <c r="A190" s="13" t="s">
         <v>279</v>
       </c>
@@ -18608,7 +18658,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="31.2">
+    <row r="191" spans="1:2" ht="31.5">
       <c r="A191" s="13" t="s">
         <v>280</v>
       </c>
@@ -18616,7 +18666,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="31.2">
+    <row r="192" spans="1:2" ht="31.5">
       <c r="A192" s="13" t="s">
         <v>281</v>
       </c>
@@ -18624,7 +18674,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="31.2">
+    <row r="193" spans="1:2" ht="31.5">
       <c r="A193" s="13" t="s">
         <v>282</v>
       </c>
@@ -18632,7 +18682,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="31.2">
+    <row r="194" spans="1:2" ht="31.5">
       <c r="A194" s="13" t="s">
         <v>283</v>
       </c>
@@ -18640,7 +18690,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="31.2">
+    <row r="195" spans="1:2" ht="31.5">
       <c r="A195" s="13" t="s">
         <v>284</v>
       </c>
@@ -18648,7 +18698,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="31.2">
+    <row r="196" spans="1:2" ht="31.5">
       <c r="A196" s="13" t="s">
         <v>285</v>
       </c>
@@ -18656,7 +18706,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="31.2">
+    <row r="197" spans="1:2" ht="31.5">
       <c r="A197" s="13" t="s">
         <v>286</v>
       </c>
@@ -18664,7 +18714,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="31.2">
+    <row r="198" spans="1:2" ht="31.5">
       <c r="A198" s="13" t="s">
         <v>287</v>
       </c>
@@ -18672,7 +18722,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="31.2">
+    <row r="199" spans="1:2" ht="31.5">
       <c r="A199" s="13" t="s">
         <v>288</v>
       </c>
@@ -18680,7 +18730,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="31.2">
+    <row r="200" spans="1:2" ht="31.5">
       <c r="A200" s="13" t="s">
         <v>289</v>
       </c>
@@ -18688,7 +18738,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="31.2">
+    <row r="201" spans="1:2" ht="31.5">
       <c r="A201" s="13" t="s">
         <v>176</v>
       </c>
@@ -18704,7 +18754,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="31.2">
+    <row r="203" spans="1:2" ht="31.5">
       <c r="A203" s="13" t="s">
         <v>83</v>
       </c>
@@ -18712,7 +18762,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="31.2">
+    <row r="204" spans="1:2" ht="31.5">
       <c r="A204" s="13" t="s">
         <v>187</v>
       </c>
@@ -18720,7 +18770,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="31.2">
+    <row r="205" spans="1:2" ht="31.5">
       <c r="A205" s="13" t="s">
         <v>188</v>
       </c>
@@ -18728,7 +18778,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="31.2">
+    <row r="206" spans="1:2" ht="31.5">
       <c r="A206" s="13" t="s">
         <v>189</v>
       </c>
@@ -18736,7 +18786,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="31.2">
+    <row r="207" spans="1:2" ht="31.5">
       <c r="A207" s="13" t="s">
         <v>84</v>
       </c>
@@ -18744,7 +18794,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="31.2">
+    <row r="208" spans="1:2" ht="31.5">
       <c r="A208" s="13" t="s">
         <v>190</v>
       </c>
@@ -18752,7 +18802,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="31.2">
+    <row r="209" spans="1:2" ht="31.5">
       <c r="A209" s="13" t="s">
         <v>253</v>
       </c>
@@ -18760,7 +18810,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="31.2">
+    <row r="210" spans="1:2" ht="31.5">
       <c r="A210" s="13" t="s">
         <v>254</v>
       </c>
@@ -18768,7 +18818,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="31.2">
+    <row r="211" spans="1:2" ht="31.5">
       <c r="A211" s="13" t="s">
         <v>255</v>
       </c>
@@ -18776,7 +18826,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="31.2">
+    <row r="212" spans="1:2" ht="31.5">
       <c r="A212" s="13" t="s">
         <v>256</v>
       </c>
@@ -18784,7 +18834,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="31.2">
+    <row r="213" spans="1:2" ht="31.5">
       <c r="A213" s="13" t="s">
         <v>257</v>
       </c>
@@ -18792,7 +18842,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="31.2">
+    <row r="214" spans="1:2" ht="31.5">
       <c r="A214" s="13" t="s">
         <v>258</v>
       </c>
@@ -18800,7 +18850,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="215" spans="1:2" s="19" customFormat="1" ht="31.2">
+    <row r="215" spans="1:2" s="19" customFormat="1" ht="31.5">
       <c r="A215" s="13" t="s">
         <v>259</v>
       </c>
@@ -18808,7 +18858,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="31.2">
+    <row r="216" spans="1:2" ht="31.5">
       <c r="A216" s="13" t="s">
         <v>260</v>
       </c>
@@ -18816,7 +18866,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="31.2">
+    <row r="217" spans="1:2" ht="31.5">
       <c r="A217" s="13" t="s">
         <v>213</v>
       </c>
@@ -18824,7 +18874,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="31.2">
+    <row r="218" spans="1:2" ht="31.5">
       <c r="A218" s="13" t="s">
         <v>290</v>
       </c>
@@ -18832,7 +18882,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="31.2">
+    <row r="219" spans="1:2" ht="31.5">
       <c r="A219" s="13" t="s">
         <v>291</v>
       </c>
@@ -18840,7 +18890,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="31.2">
+    <row r="220" spans="1:2" ht="31.5">
       <c r="A220" s="13" t="s">
         <v>292</v>
       </c>
@@ -18848,7 +18898,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="31.2">
+    <row r="221" spans="1:2" ht="31.5">
       <c r="A221" s="13" t="s">
         <v>293</v>
       </c>
@@ -18856,7 +18906,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="31.2">
+    <row r="222" spans="1:2" ht="31.5">
       <c r="A222" s="13" t="s">
         <v>294</v>
       </c>
@@ -18864,7 +18914,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="31.2">
+    <row r="223" spans="1:2" ht="31.5">
       <c r="A223" s="13" t="s">
         <v>295</v>
       </c>
@@ -18872,7 +18922,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="31.2">
+    <row r="224" spans="1:2" ht="31.5">
       <c r="A224" s="13" t="s">
         <v>296</v>
       </c>
@@ -18880,7 +18930,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="31.2">
+    <row r="225" spans="1:2" ht="31.5">
       <c r="A225" s="13" t="s">
         <v>297</v>
       </c>
@@ -19014,7 +19064,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="30">
+    <row r="242" spans="1:2" ht="45">
       <c r="A242" s="14" t="s">
         <v>87</v>
       </c>
@@ -19022,7 +19072,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="30">
+    <row r="243" spans="1:2" ht="45">
       <c r="A243" s="14" t="s">
         <v>88</v>
       </c>
@@ -19046,7 +19096,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="30">
+    <row r="246" spans="1:2" ht="45">
       <c r="A246" s="14" t="s">
         <v>87</v>
       </c>
@@ -19054,7 +19104,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="30">
+    <row r="247" spans="1:2" ht="45">
       <c r="A247" s="14" t="s">
         <v>88</v>
       </c>
@@ -19097,91 +19147,91 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:HY18"/>
+  <dimension ref="A1:IK18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="GO1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="HT2" sqref="HT2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="4" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="4" width="11.28515625" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" customWidth="1"/>
-    <col min="18" max="18" width="9.33203125" customWidth="1"/>
-    <col min="22" max="22" width="10.6640625" customWidth="1"/>
-    <col min="23" max="23" width="10.33203125" customWidth="1"/>
-    <col min="24" max="24" width="10.109375" customWidth="1"/>
-    <col min="25" max="25" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" customWidth="1"/>
     <col min="26" max="26" width="10" customWidth="1"/>
     <col min="27" max="27" width="11" customWidth="1"/>
     <col min="29" max="29" width="11" customWidth="1"/>
-    <col min="30" max="30" width="13.88671875" customWidth="1"/>
-    <col min="31" max="31" width="10.44140625" customWidth="1"/>
-    <col min="32" max="32" width="13.88671875" customWidth="1"/>
-    <col min="33" max="35" width="13.33203125" customWidth="1"/>
-    <col min="36" max="36" width="10.33203125" customWidth="1"/>
-    <col min="37" max="37" width="11.44140625" customWidth="1"/>
-    <col min="38" max="38" width="10.6640625" customWidth="1"/>
-    <col min="39" max="39" width="9.88671875" customWidth="1"/>
-    <col min="42" max="43" width="10.33203125" customWidth="1"/>
-    <col min="44" max="44" width="11.5546875" customWidth="1"/>
+    <col min="30" max="30" width="13.85546875" customWidth="1"/>
+    <col min="31" max="31" width="10.42578125" customWidth="1"/>
+    <col min="32" max="32" width="13.85546875" customWidth="1"/>
+    <col min="33" max="35" width="13.28515625" customWidth="1"/>
+    <col min="36" max="36" width="10.28515625" customWidth="1"/>
+    <col min="37" max="37" width="11.42578125" customWidth="1"/>
+    <col min="38" max="38" width="10.7109375" customWidth="1"/>
+    <col min="39" max="39" width="9.85546875" customWidth="1"/>
+    <col min="42" max="43" width="10.28515625" customWidth="1"/>
+    <col min="44" max="44" width="11.5703125" customWidth="1"/>
     <col min="45" max="45" width="14" customWidth="1"/>
-    <col min="46" max="46" width="10.44140625" customWidth="1"/>
-    <col min="47" max="47" width="11.5546875" customWidth="1"/>
-    <col min="48" max="48" width="13.33203125" customWidth="1"/>
-    <col min="49" max="49" width="11.44140625" customWidth="1"/>
-    <col min="50" max="52" width="10.33203125" customWidth="1"/>
+    <col min="46" max="46" width="10.42578125" customWidth="1"/>
+    <col min="47" max="47" width="11.5703125" customWidth="1"/>
+    <col min="48" max="48" width="13.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.42578125" customWidth="1"/>
+    <col min="50" max="52" width="10.28515625" customWidth="1"/>
     <col min="53" max="53" width="11" customWidth="1"/>
-    <col min="54" max="54" width="12.6640625" customWidth="1"/>
-    <col min="55" max="65" width="9.6640625" customWidth="1"/>
-    <col min="66" max="66" width="15.6640625" customWidth="1"/>
-    <col min="67" max="68" width="12.6640625" customWidth="1"/>
-    <col min="69" max="70" width="14.5546875" customWidth="1"/>
-    <col min="85" max="85" width="11.33203125" customWidth="1"/>
-    <col min="86" max="86" width="11.5546875" customWidth="1"/>
+    <col min="54" max="54" width="12.7109375" customWidth="1"/>
+    <col min="55" max="65" width="9.7109375" customWidth="1"/>
+    <col min="66" max="66" width="15.7109375" customWidth="1"/>
+    <col min="67" max="68" width="12.7109375" customWidth="1"/>
+    <col min="69" max="70" width="14.5703125" customWidth="1"/>
+    <col min="85" max="85" width="11.28515625" customWidth="1"/>
+    <col min="86" max="86" width="11.5703125" customWidth="1"/>
     <col min="87" max="87" width="11" customWidth="1"/>
-    <col min="88" max="88" width="10.88671875" customWidth="1"/>
-    <col min="89" max="89" width="10.6640625" customWidth="1"/>
-    <col min="92" max="92" width="13.109375" customWidth="1"/>
-    <col min="97" max="97" width="13.6640625" customWidth="1"/>
-    <col min="98" max="98" width="12.6640625" customWidth="1"/>
-    <col min="99" max="99" width="11.33203125" customWidth="1"/>
+    <col min="88" max="88" width="10.85546875" customWidth="1"/>
+    <col min="89" max="89" width="10.7109375" customWidth="1"/>
+    <col min="92" max="92" width="13.140625" customWidth="1"/>
+    <col min="97" max="97" width="13.7109375" customWidth="1"/>
+    <col min="98" max="98" width="12.7109375" customWidth="1"/>
+    <col min="99" max="99" width="11.28515625" customWidth="1"/>
     <col min="103" max="103" width="10" customWidth="1"/>
-    <col min="104" max="104" width="11.6640625" customWidth="1"/>
-    <col min="111" max="111" width="10.5546875" customWidth="1"/>
+    <col min="104" max="104" width="11.7109375" customWidth="1"/>
+    <col min="111" max="111" width="10.5703125" customWidth="1"/>
     <col min="114" max="114" width="10" customWidth="1"/>
-    <col min="115" max="115" width="10.33203125" customWidth="1"/>
-    <col min="116" max="116" width="10.88671875" customWidth="1"/>
-    <col min="117" max="118" width="10.6640625" customWidth="1"/>
-    <col min="119" max="119" width="10.88671875" customWidth="1"/>
-    <col min="120" max="120" width="10.6640625" customWidth="1"/>
-    <col min="121" max="121" width="11.33203125" customWidth="1"/>
-    <col min="122" max="122" width="14.6640625" customWidth="1"/>
-    <col min="123" max="123" width="14.88671875" customWidth="1"/>
-    <col min="124" max="124" width="13.5546875" customWidth="1"/>
-    <col min="127" max="127" width="11.109375" customWidth="1"/>
-    <col min="131" max="132" width="9.5546875" customWidth="1"/>
-    <col min="133" max="133" width="10.109375" customWidth="1"/>
-    <col min="134" max="135" width="10.33203125" customWidth="1"/>
-    <col min="136" max="136" width="9.6640625" customWidth="1"/>
-    <col min="137" max="137" width="11.109375" customWidth="1"/>
-    <col min="138" max="138" width="9.6640625" customWidth="1"/>
-    <col min="139" max="139" width="10.88671875" customWidth="1"/>
-    <col min="140" max="141" width="9.6640625" customWidth="1"/>
-    <col min="142" max="143" width="10.33203125" customWidth="1"/>
-    <col min="144" max="144" width="9.6640625" customWidth="1"/>
-    <col min="159" max="159" width="11.109375" customWidth="1"/>
-    <col min="190" max="190" width="11.6640625" customWidth="1"/>
-    <col min="216" max="216" width="11.5546875" customWidth="1"/>
-    <col min="217" max="217" width="13.44140625" customWidth="1"/>
-    <col min="218" max="219" width="10.88671875" customWidth="1"/>
-    <col min="220" max="227" width="8.88671875" style="39"/>
+    <col min="115" max="115" width="10.28515625" customWidth="1"/>
+    <col min="116" max="116" width="10.85546875" customWidth="1"/>
+    <col min="117" max="118" width="10.7109375" customWidth="1"/>
+    <col min="119" max="119" width="10.85546875" customWidth="1"/>
+    <col min="120" max="120" width="10.7109375" customWidth="1"/>
+    <col min="121" max="121" width="11.28515625" customWidth="1"/>
+    <col min="122" max="122" width="14.7109375" customWidth="1"/>
+    <col min="123" max="123" width="14.85546875" customWidth="1"/>
+    <col min="124" max="124" width="13.5703125" customWidth="1"/>
+    <col min="127" max="127" width="11.140625" customWidth="1"/>
+    <col min="131" max="132" width="9.5703125" customWidth="1"/>
+    <col min="133" max="133" width="10.140625" customWidth="1"/>
+    <col min="134" max="135" width="10.28515625" customWidth="1"/>
+    <col min="136" max="136" width="9.7109375" customWidth="1"/>
+    <col min="137" max="137" width="11.140625" customWidth="1"/>
+    <col min="138" max="138" width="9.7109375" customWidth="1"/>
+    <col min="139" max="139" width="10.85546875" customWidth="1"/>
+    <col min="140" max="141" width="9.7109375" customWidth="1"/>
+    <col min="142" max="143" width="10.28515625" customWidth="1"/>
+    <col min="144" max="144" width="9.7109375" customWidth="1"/>
+    <col min="159" max="159" width="11.140625" customWidth="1"/>
+    <col min="190" max="190" width="11.7109375" customWidth="1"/>
+    <col min="216" max="216" width="11.5703125" customWidth="1"/>
+    <col min="217" max="217" width="13.42578125" customWidth="1"/>
+    <col min="218" max="219" width="10.85546875" customWidth="1"/>
+    <col min="220" max="239" width="8.85546875" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:233" s="43" customFormat="1" ht="26.25" customHeight="1">
+    <row r="1" spans="1:245" s="43" customFormat="1" ht="26.25" customHeight="1">
       <c r="A1" s="44" t="s">
         <v>262</v>
       </c>
@@ -19193,8 +19243,20 @@
       <c r="HQ1" s="47"/>
       <c r="HR1" s="47"/>
       <c r="HS1" s="47"/>
-    </row>
-    <row r="2" spans="1:233" s="33" customFormat="1" ht="144.6" customHeight="1">
+      <c r="HT1" s="47"/>
+      <c r="HU1" s="47"/>
+      <c r="HV1" s="47"/>
+      <c r="HW1" s="47"/>
+      <c r="HX1" s="47"/>
+      <c r="HY1" s="47"/>
+      <c r="HZ1" s="47"/>
+      <c r="IA1" s="47"/>
+      <c r="IB1" s="47"/>
+      <c r="IC1" s="47"/>
+      <c r="ID1" s="47"/>
+      <c r="IE1" s="47"/>
+    </row>
+    <row r="2" spans="1:245" s="33" customFormat="1" ht="144.6" customHeight="1">
       <c r="A2" s="21" t="s">
         <v>13</v>
       </c>
@@ -19790,7 +19852,7 @@
         <v>297</v>
       </c>
       <c r="GQ2" s="13" t="s">
-        <v>137</v>
+        <v>342</v>
       </c>
       <c r="GR2" s="55" t="s">
         <v>335</v>
@@ -19847,7 +19909,7 @@
         <v>307</v>
       </c>
       <c r="HJ2" s="54" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="HK2" s="54" t="s">
         <v>334</v>
@@ -19877,25 +19939,61 @@
         <v>329</v>
       </c>
       <c r="HT2" s="50" t="s">
+        <v>344</v>
+      </c>
+      <c r="HU2" s="50" t="s">
+        <v>345</v>
+      </c>
+      <c r="HV2" s="50" t="s">
+        <v>346</v>
+      </c>
+      <c r="HW2" s="50" t="s">
+        <v>347</v>
+      </c>
+      <c r="HX2" s="50" t="s">
+        <v>348</v>
+      </c>
+      <c r="HY2" s="50" t="s">
+        <v>349</v>
+      </c>
+      <c r="HZ2" s="50" t="s">
+        <v>350</v>
+      </c>
+      <c r="IA2" s="50" t="s">
+        <v>351</v>
+      </c>
+      <c r="IB2" s="50" t="s">
+        <v>352</v>
+      </c>
+      <c r="IC2" s="50" t="s">
+        <v>353</v>
+      </c>
+      <c r="ID2" s="50" t="s">
+        <v>354</v>
+      </c>
+      <c r="IE2" s="50" t="s">
+        <v>355</v>
+      </c>
+      <c r="IF2" s="50" t="s">
         <v>319</v>
       </c>
-      <c r="HU2" s="50" t="s">
+      <c r="IG2" s="50" t="s">
         <v>320</v>
       </c>
-      <c r="HV2" s="50" t="s">
+      <c r="IH2" s="50" t="s">
         <v>321</v>
       </c>
-      <c r="HW2" s="50" t="s">
+      <c r="II2" s="50" t="s">
         <v>322</v>
       </c>
-      <c r="HX2" s="50" t="s">
+      <c r="IJ2" s="50" t="s">
         <v>323</v>
       </c>
-      <c r="HY2" s="13" t="s">
+      <c r="IK2" s="13" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:233" s="33" customFormat="1" ht="164.4" customHeight="1">
+    <row r="3" spans="1:245" s="33" customFormat="1" ht="164.45" customHeight="1">
       <c r="A3" s="34" t="s">
         <v>1</v>
       </c>
@@ -20559,38 +20657,50 @@
       <c r="HS3" s="50" t="s">
         <v>331</v>
       </c>
-      <c r="HT3" s="50" t="s">
+      <c r="HT3" s="50"/>
+      <c r="HU3" s="50"/>
+      <c r="HV3" s="50"/>
+      <c r="HW3" s="50"/>
+      <c r="HX3" s="50"/>
+      <c r="HY3" s="50"/>
+      <c r="HZ3" s="50"/>
+      <c r="IA3" s="50"/>
+      <c r="IB3" s="50"/>
+      <c r="IC3" s="50"/>
+      <c r="ID3" s="50"/>
+      <c r="IE3" s="50"/>
+      <c r="IF3" s="50" t="s">
         <v>319</v>
       </c>
-      <c r="HU3" s="50" t="s">
+      <c r="IG3" s="50" t="s">
         <v>320</v>
       </c>
-      <c r="HV3" s="50" t="s">
+      <c r="IH3" s="50" t="s">
         <v>321</v>
       </c>
-      <c r="HW3" s="50" t="s">
+      <c r="II3" s="50" t="s">
         <v>322</v>
       </c>
-      <c r="HX3" s="50" t="s">
+      <c r="IJ3" s="50" t="s">
         <v>323</v>
       </c>
-      <c r="HY3" s="34" t="s">
+      <c r="IK3" s="34" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:233" s="33" customFormat="1"/>
-    <row r="5" spans="1:233" s="33" customFormat="1"/>
-    <row r="6" spans="1:233" s="33" customFormat="1"/>
-    <row r="7" spans="1:233" s="33" customFormat="1"/>
-    <row r="8" spans="1:233" s="33" customFormat="1"/>
-    <row r="9" spans="1:233" s="33" customFormat="1"/>
-    <row r="10" spans="1:233" s="33" customFormat="1"/>
-    <row r="11" spans="1:233" s="33" customFormat="1"/>
-    <row r="12" spans="1:233" s="33" customFormat="1"/>
-    <row r="13" spans="1:233" s="39" customFormat="1"/>
-    <row r="14" spans="1:233" s="39" customFormat="1"/>
-    <row r="15" spans="1:233" s="39" customFormat="1"/>
-    <row r="16" spans="1:233" s="39" customFormat="1"/>
+    <row r="4" spans="1:245" s="33" customFormat="1"/>
+    <row r="5" spans="1:245" s="33" customFormat="1"/>
+    <row r="6" spans="1:245" s="33" customFormat="1"/>
+    <row r="7" spans="1:245" s="33" customFormat="1"/>
+    <row r="8" spans="1:245" s="33" customFormat="1"/>
+    <row r="9" spans="1:245" s="33" customFormat="1"/>
+    <row r="10" spans="1:245" s="33" customFormat="1"/>
+    <row r="11" spans="1:245" s="33" customFormat="1"/>
+    <row r="12" spans="1:245" s="33" customFormat="1"/>
+    <row r="13" spans="1:245" s="39" customFormat="1"/>
+    <row r="14" spans="1:245" s="39" customFormat="1"/>
+    <row r="15" spans="1:245" s="39" customFormat="1"/>
+    <row r="16" spans="1:245" s="39" customFormat="1"/>
     <row r="17" s="39" customFormat="1"/>
     <row r="18" s="39" customFormat="1"/>
   </sheetData>

</xml_diff>